<commit_message>
add book bulk with excel
</commit_message>
<xml_diff>
--- a/booklist.xlsx
+++ b/booklist.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgoh/Repository/geuk-small-library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CEE6B-1068-6F41-AC9E-6C3084C4F5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F1965-271C-F04B-8726-ECAF5021E962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="820" windowWidth="28300" windowHeight="17440" activeTab="1" xr2:uid="{A0C61242-67DC-074B-9286-D9D7858EF7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="mySheet" sheetId="2" r:id="rId2"/>
+    <sheet name="GEUK 도서 리스트" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>no.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,30 @@
   </si>
   <si>
     <t>test4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Author</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Released Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분실여부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,64 +599,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C340847-264C-FB47-96AF-9F81E626B7D3}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="B1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="2:7">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="b">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44177</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>